<commit_message>
Fixed time period with more than 4 years
</commit_message>
<xml_diff>
--- a/lattes_qualis/coleta_bruno_araujo_CC.xlsx
+++ b/lattes_qualis/coleta_bruno_araujo_CC.xlsx
@@ -1,34 +1,34 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
-    <workbookView activeTab="0" autoFilterDateGrouping="1" firstSheet="0" minimized="0" showHorizontalScroll="1" showSheetTabs="1" showVerticalScroll="1" tabRatio="600" visibility="visible"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Parâmetros" sheetId="1" state="visible" r:id="rId1"/>
-    <sheet name="Indicadores" sheetId="2" state="visible" r:id="rId2"/>
-    <sheet name="Autores" sheetId="3" state="visible" r:id="rId3"/>
-    <sheet name="Art|PPG" sheetId="4" state="visible" r:id="rId4"/>
-    <sheet name="Gráficos Q2016" sheetId="5" state="visible" r:id="rId5"/>
-    <sheet name="Gráficos Q2019" sheetId="6" state="visible" r:id="rId6"/>
-    <sheet name="Resumo Q2016" sheetId="7" state="visible" r:id="rId7"/>
-    <sheet name="Resumo Q2019" sheetId="8" state="visible" r:id="rId8"/>
-    <sheet name="Art|Prof" sheetId="9" state="visible" r:id="rId9"/>
-    <sheet name="Anais|PPG" sheetId="10" state="visible" r:id="rId10"/>
-    <sheet name="Periódicos|PPG" sheetId="11" state="visible" r:id="rId11"/>
-    <sheet name="Bruno" sheetId="12" state="visible" r:id="rId12"/>
-    <sheet name="Exceções" sheetId="13" state="visible" r:id="rId13"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Parâmetros" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Indicadores" sheetId="2" state="visible" r:id="rId2"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Autores" sheetId="3" state="visible" r:id="rId3"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Art|PPG" sheetId="4" state="visible" r:id="rId4"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Gráficos Q2016" sheetId="5" state="visible" r:id="rId5"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Gráficos Q2019" sheetId="6" state="visible" r:id="rId6"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Resumo Q2016" sheetId="7" state="visible" r:id="rId7"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Resumo Q2019" sheetId="8" state="visible" r:id="rId8"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Art|Prof" sheetId="9" state="visible" r:id="rId9"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Anais|PPG" sheetId="10" state="visible" r:id="rId10"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Periódicos|PPG" sheetId="11" state="visible" r:id="rId11"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Bruno" sheetId="12" state="visible" r:id="rId12"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Exceções" sheetId="13" state="visible" r:id="rId13"/>
   </sheets>
   <definedNames>
-    <definedName hidden="1" localSheetId="2" name="_xlnm._FilterDatabase">'Autores'!$A$1:$G$66</definedName>
-    <definedName hidden="1" localSheetId="3" name="_xlnm._FilterDatabase">'Art|PPG'!$A$1:$V$23</definedName>
-    <definedName hidden="1" localSheetId="8" name="_xlnm._FilterDatabase">'Art|Prof'!$A$1:$V$31</definedName>
-    <definedName hidden="1" localSheetId="9" name="_xlnm._FilterDatabase">'Anais|PPG'!$A$1:$F$3</definedName>
-    <definedName hidden="1" localSheetId="10" name="_xlnm._FilterDatabase">'Periódicos|PPG'!$A$1:$G$23</definedName>
-    <definedName hidden="1" localSheetId="11" name="_xlnm._FilterDatabase">'Bruno'!$A$1:$U$31</definedName>
-    <definedName hidden="1" localSheetId="12" name="_xlnm._FilterDatabase">'Exceções'!$A$1:$C$1</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">'Autores'!$A$1:$G$66</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">'Art|PPG'!$A$1:$V$23</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="8" hidden="1">'Art|Prof'!$A$1:$V$31</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="9" hidden="1">'Anais|PPG'!$A$1:$F$3</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="10" hidden="1">'Periódicos|PPG'!$A$1:$G$23</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="11" hidden="1">'Bruno'!$A$1:$U$31</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="12" hidden="1">'Exceções'!$A$1:$C$1</definedName>
   </definedNames>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
@@ -188,77 +188,77 @@
     </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="25">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf applyAlignment="1" borderId="1" fillId="0" fontId="1" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf applyAlignment="1" borderId="1" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf applyAlignment="1" borderId="0" fillId="4" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf applyAlignment="1" borderId="0" fillId="4" fontId="1" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf borderId="0" fillId="4" fontId="1" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf borderId="1" fillId="0" fontId="1" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf borderId="1" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf borderId="0" fillId="4" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf applyAlignment="1" borderId="1" fillId="5" fontId="2" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf applyAlignment="1" borderId="1" fillId="6" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf applyAlignment="1" borderId="1" fillId="2" fontId="1" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf applyAlignment="1" borderId="1" fillId="3" fontId="2" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf applyAlignment="1" borderId="1" fillId="2" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf applyAlignment="1" borderId="0" fillId="0" fontId="1" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf applyAlignment="1" borderId="1" fillId="4" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf applyAlignment="1" borderId="1" fillId="7" fontId="3" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf applyAlignment="1" borderId="1" fillId="8" fontId="1" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf applyAlignment="1" borderId="1" fillId="8" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf applyAlignment="1" borderId="0" fillId="4" fontId="3" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf applyAlignment="1" borderId="6" fillId="4" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="6" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf applyAlignment="1" borderId="6" fillId="0" fontId="1" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf applyAlignment="1" borderId="6" fillId="4" fontId="3" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="6" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf applyAlignment="1" borderId="0" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle builtinId="0" hidden="0" name="Normal" xfId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
   </cellStyles>
-  <tableStyles count="0" defaultPivotStyle="PivotStyleLight16" defaultTableStyle="TableStyleMedium9"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
     <indexedColors>
       <rgbColor rgb="00000000"/>
@@ -331,7 +331,7 @@
 </file>
 
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
-<wsDr xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
+<wsDr xmlns="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
   <oneCellAnchor>
     <from>
       <col>0</col>
@@ -342,17 +342,17 @@
     <ext cx="5715000" cy="3429000"/>
     <pic>
       <nvPicPr>
-        <cNvPr descr="Picture" id="1" name="Image 1"/>
+        <cNvPr id="1" name="Image 1" descr="Picture"/>
         <cNvPicPr/>
       </nvPicPr>
       <blipFill>
-        <a:blip cstate="print" r:embed="rId1"/>
-        <a:stretch>
+        <a:blip xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" cstate="print" r:embed="rId1"/>
+        <a:stretch xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
           <a:fillRect/>
         </a:stretch>
       </blipFill>
       <spPr>
-        <a:prstGeom prst="rect"/>
+        <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="rect"/>
       </spPr>
     </pic>
     <clientData/>
@@ -367,17 +367,17 @@
     <ext cx="5715000" cy="3429000"/>
     <pic>
       <nvPicPr>
-        <cNvPr descr="Picture" id="2" name="Image 2"/>
+        <cNvPr id="2" name="Image 2" descr="Picture"/>
         <cNvPicPr/>
       </nvPicPr>
       <blipFill>
-        <a:blip cstate="print" r:embed="rId2"/>
-        <a:stretch>
+        <a:blip xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" cstate="print" r:embed="rId2"/>
+        <a:stretch xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
           <a:fillRect/>
         </a:stretch>
       </blipFill>
       <spPr>
-        <a:prstGeom prst="rect"/>
+        <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="rect"/>
       </spPr>
     </pic>
     <clientData/>
@@ -392,17 +392,17 @@
     <ext cx="5715000" cy="3429000"/>
     <pic>
       <nvPicPr>
-        <cNvPr descr="Picture" id="3" name="Image 3"/>
+        <cNvPr id="3" name="Image 3" descr="Picture"/>
         <cNvPicPr/>
       </nvPicPr>
       <blipFill>
-        <a:blip cstate="print" r:embed="rId3"/>
-        <a:stretch>
+        <a:blip xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" cstate="print" r:embed="rId3"/>
+        <a:stretch xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
           <a:fillRect/>
         </a:stretch>
       </blipFill>
       <spPr>
-        <a:prstGeom prst="rect"/>
+        <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="rect"/>
       </spPr>
     </pic>
     <clientData/>
@@ -417,17 +417,17 @@
     <ext cx="5715000" cy="3429000"/>
     <pic>
       <nvPicPr>
-        <cNvPr descr="Picture" id="4" name="Image 4"/>
+        <cNvPr id="4" name="Image 4" descr="Picture"/>
         <cNvPicPr/>
       </nvPicPr>
       <blipFill>
-        <a:blip cstate="print" r:embed="rId4"/>
-        <a:stretch>
+        <a:blip xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" cstate="print" r:embed="rId4"/>
+        <a:stretch xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
           <a:fillRect/>
         </a:stretch>
       </blipFill>
       <spPr>
-        <a:prstGeom prst="rect"/>
+        <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="rect"/>
       </spPr>
     </pic>
     <clientData/>
@@ -442,17 +442,17 @@
     <ext cx="5715000" cy="3429000"/>
     <pic>
       <nvPicPr>
-        <cNvPr descr="Picture" id="5" name="Image 5"/>
+        <cNvPr id="5" name="Image 5" descr="Picture"/>
         <cNvPicPr/>
       </nvPicPr>
       <blipFill>
-        <a:blip cstate="print" r:embed="rId5"/>
-        <a:stretch>
+        <a:blip xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" cstate="print" r:embed="rId5"/>
+        <a:stretch xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
           <a:fillRect/>
         </a:stretch>
       </blipFill>
       <spPr>
-        <a:prstGeom prst="rect"/>
+        <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="rect"/>
       </spPr>
     </pic>
     <clientData/>
@@ -467,17 +467,17 @@
     <ext cx="5715000" cy="3429000"/>
     <pic>
       <nvPicPr>
-        <cNvPr descr="Picture" id="6" name="Image 6"/>
+        <cNvPr id="6" name="Image 6" descr="Picture"/>
         <cNvPicPr/>
       </nvPicPr>
       <blipFill>
-        <a:blip cstate="print" r:embed="rId6"/>
-        <a:stretch>
+        <a:blip xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" cstate="print" r:embed="rId6"/>
+        <a:stretch xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
           <a:fillRect/>
         </a:stretch>
       </blipFill>
       <spPr>
-        <a:prstGeom prst="rect"/>
+        <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="rect"/>
       </spPr>
     </pic>
     <clientData/>
@@ -492,17 +492,17 @@
     <ext cx="5715000" cy="3429000"/>
     <pic>
       <nvPicPr>
-        <cNvPr descr="Picture" id="7" name="Image 7"/>
+        <cNvPr id="7" name="Image 7" descr="Picture"/>
         <cNvPicPr/>
       </nvPicPr>
       <blipFill>
-        <a:blip cstate="print" r:embed="rId7"/>
-        <a:stretch>
+        <a:blip xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" cstate="print" r:embed="rId7"/>
+        <a:stretch xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
           <a:fillRect/>
         </a:stretch>
       </blipFill>
       <spPr>
-        <a:prstGeom prst="rect"/>
+        <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="rect"/>
       </spPr>
     </pic>
     <clientData/>
@@ -517,17 +517,17 @@
     <ext cx="5715000" cy="3429000"/>
     <pic>
       <nvPicPr>
-        <cNvPr descr="Picture" id="8" name="Image 8"/>
+        <cNvPr id="8" name="Image 8" descr="Picture"/>
         <cNvPicPr/>
       </nvPicPr>
       <blipFill>
-        <a:blip cstate="print" r:embed="rId8"/>
-        <a:stretch>
+        <a:blip xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" cstate="print" r:embed="rId8"/>
+        <a:stretch xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
           <a:fillRect/>
         </a:stretch>
       </blipFill>
       <spPr>
-        <a:prstGeom prst="rect"/>
+        <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="rect"/>
       </spPr>
     </pic>
     <clientData/>
@@ -542,17 +542,17 @@
     <ext cx="5715000" cy="3429000"/>
     <pic>
       <nvPicPr>
-        <cNvPr descr="Picture" id="9" name="Image 9"/>
+        <cNvPr id="9" name="Image 9" descr="Picture"/>
         <cNvPicPr/>
       </nvPicPr>
       <blipFill>
-        <a:blip cstate="print" r:embed="rId9"/>
-        <a:stretch>
+        <a:blip xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" cstate="print" r:embed="rId9"/>
+        <a:stretch xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
           <a:fillRect/>
         </a:stretch>
       </blipFill>
       <spPr>
-        <a:prstGeom prst="rect"/>
+        <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="rect"/>
       </spPr>
     </pic>
     <clientData/>
@@ -567,17 +567,17 @@
     <ext cx="5715000" cy="3429000"/>
     <pic>
       <nvPicPr>
-        <cNvPr descr="Picture" id="10" name="Image 10"/>
+        <cNvPr id="10" name="Image 10" descr="Picture"/>
         <cNvPicPr/>
       </nvPicPr>
       <blipFill>
-        <a:blip cstate="print" r:embed="rId10"/>
-        <a:stretch>
+        <a:blip xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" cstate="print" r:embed="rId10"/>
+        <a:stretch xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
           <a:fillRect/>
         </a:stretch>
       </blipFill>
       <spPr>
-        <a:prstGeom prst="rect"/>
+        <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="rect"/>
       </spPr>
     </pic>
     <clientData/>
@@ -592,17 +592,17 @@
     <ext cx="5715000" cy="3429000"/>
     <pic>
       <nvPicPr>
-        <cNvPr descr="Picture" id="11" name="Image 11"/>
+        <cNvPr id="11" name="Image 11" descr="Picture"/>
         <cNvPicPr/>
       </nvPicPr>
       <blipFill>
-        <a:blip cstate="print" r:embed="rId11"/>
-        <a:stretch>
+        <a:blip xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" cstate="print" r:embed="rId11"/>
+        <a:stretch xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
           <a:fillRect/>
         </a:stretch>
       </blipFill>
       <spPr>
-        <a:prstGeom prst="rect"/>
+        <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="rect"/>
       </spPr>
     </pic>
     <clientData/>
@@ -617,17 +617,17 @@
     <ext cx="5715000" cy="3429000"/>
     <pic>
       <nvPicPr>
-        <cNvPr descr="Picture" id="12" name="Image 12"/>
+        <cNvPr id="12" name="Image 12" descr="Picture"/>
         <cNvPicPr/>
       </nvPicPr>
       <blipFill>
-        <a:blip cstate="print" r:embed="rId12"/>
-        <a:stretch>
+        <a:blip xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" cstate="print" r:embed="rId12"/>
+        <a:stretch xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
           <a:fillRect/>
         </a:stretch>
       </blipFill>
       <spPr>
-        <a:prstGeom prst="rect"/>
+        <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="rect"/>
       </spPr>
     </pic>
     <clientData/>
@@ -636,7 +636,7 @@
 </file>
 
 <file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
-<wsDr xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
+<wsDr xmlns="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
   <oneCellAnchor>
     <from>
       <col>0</col>
@@ -647,17 +647,17 @@
     <ext cx="5715000" cy="3429000"/>
     <pic>
       <nvPicPr>
-        <cNvPr descr="Picture" id="1" name="Image 1"/>
+        <cNvPr id="1" name="Image 1" descr="Picture"/>
         <cNvPicPr/>
       </nvPicPr>
       <blipFill>
-        <a:blip cstate="print" r:embed="rId1"/>
-        <a:stretch>
+        <a:blip xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" cstate="print" r:embed="rId1"/>
+        <a:stretch xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
           <a:fillRect/>
         </a:stretch>
       </blipFill>
       <spPr>
-        <a:prstGeom prst="rect"/>
+        <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="rect"/>
       </spPr>
     </pic>
     <clientData/>
@@ -672,17 +672,17 @@
     <ext cx="5715000" cy="3429000"/>
     <pic>
       <nvPicPr>
-        <cNvPr descr="Picture" id="2" name="Image 2"/>
+        <cNvPr id="2" name="Image 2" descr="Picture"/>
         <cNvPicPr/>
       </nvPicPr>
       <blipFill>
-        <a:blip cstate="print" r:embed="rId2"/>
-        <a:stretch>
+        <a:blip xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" cstate="print" r:embed="rId2"/>
+        <a:stretch xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
           <a:fillRect/>
         </a:stretch>
       </blipFill>
       <spPr>
-        <a:prstGeom prst="rect"/>
+        <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="rect"/>
       </spPr>
     </pic>
     <clientData/>
@@ -697,17 +697,17 @@
     <ext cx="5715000" cy="3429000"/>
     <pic>
       <nvPicPr>
-        <cNvPr descr="Picture" id="3" name="Image 3"/>
+        <cNvPr id="3" name="Image 3" descr="Picture"/>
         <cNvPicPr/>
       </nvPicPr>
       <blipFill>
-        <a:blip cstate="print" r:embed="rId3"/>
-        <a:stretch>
+        <a:blip xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" cstate="print" r:embed="rId3"/>
+        <a:stretch xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
           <a:fillRect/>
         </a:stretch>
       </blipFill>
       <spPr>
-        <a:prstGeom prst="rect"/>
+        <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="rect"/>
       </spPr>
     </pic>
     <clientData/>
@@ -722,17 +722,17 @@
     <ext cx="5715000" cy="3429000"/>
     <pic>
       <nvPicPr>
-        <cNvPr descr="Picture" id="4" name="Image 4"/>
+        <cNvPr id="4" name="Image 4" descr="Picture"/>
         <cNvPicPr/>
       </nvPicPr>
       <blipFill>
-        <a:blip cstate="print" r:embed="rId4"/>
-        <a:stretch>
+        <a:blip xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" cstate="print" r:embed="rId4"/>
+        <a:stretch xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
           <a:fillRect/>
         </a:stretch>
       </blipFill>
       <spPr>
-        <a:prstGeom prst="rect"/>
+        <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="rect"/>
       </spPr>
     </pic>
     <clientData/>
@@ -747,17 +747,17 @@
     <ext cx="5715000" cy="3429000"/>
     <pic>
       <nvPicPr>
-        <cNvPr descr="Picture" id="5" name="Image 5"/>
+        <cNvPr id="5" name="Image 5" descr="Picture"/>
         <cNvPicPr/>
       </nvPicPr>
       <blipFill>
-        <a:blip cstate="print" r:embed="rId5"/>
-        <a:stretch>
+        <a:blip xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" cstate="print" r:embed="rId5"/>
+        <a:stretch xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
           <a:fillRect/>
         </a:stretch>
       </blipFill>
       <spPr>
-        <a:prstGeom prst="rect"/>
+        <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="rect"/>
       </spPr>
     </pic>
     <clientData/>
@@ -772,17 +772,17 @@
     <ext cx="5715000" cy="3429000"/>
     <pic>
       <nvPicPr>
-        <cNvPr descr="Picture" id="6" name="Image 6"/>
+        <cNvPr id="6" name="Image 6" descr="Picture"/>
         <cNvPicPr/>
       </nvPicPr>
       <blipFill>
-        <a:blip cstate="print" r:embed="rId6"/>
-        <a:stretch>
+        <a:blip xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" cstate="print" r:embed="rId6"/>
+        <a:stretch xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
           <a:fillRect/>
         </a:stretch>
       </blipFill>
       <spPr>
-        <a:prstGeom prst="rect"/>
+        <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="rect"/>
       </spPr>
     </pic>
     <clientData/>
@@ -797,17 +797,17 @@
     <ext cx="5715000" cy="3429000"/>
     <pic>
       <nvPicPr>
-        <cNvPr descr="Picture" id="7" name="Image 7"/>
+        <cNvPr id="7" name="Image 7" descr="Picture"/>
         <cNvPicPr/>
       </nvPicPr>
       <blipFill>
-        <a:blip cstate="print" r:embed="rId7"/>
-        <a:stretch>
+        <a:blip xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" cstate="print" r:embed="rId7"/>
+        <a:stretch xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
           <a:fillRect/>
         </a:stretch>
       </blipFill>
       <spPr>
-        <a:prstGeom prst="rect"/>
+        <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="rect"/>
       </spPr>
     </pic>
     <clientData/>
@@ -822,17 +822,17 @@
     <ext cx="5715000" cy="3429000"/>
     <pic>
       <nvPicPr>
-        <cNvPr descr="Picture" id="8" name="Image 8"/>
+        <cNvPr id="8" name="Image 8" descr="Picture"/>
         <cNvPicPr/>
       </nvPicPr>
       <blipFill>
-        <a:blip cstate="print" r:embed="rId8"/>
-        <a:stretch>
+        <a:blip xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" cstate="print" r:embed="rId8"/>
+        <a:stretch xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
           <a:fillRect/>
         </a:stretch>
       </blipFill>
       <spPr>
-        <a:prstGeom prst="rect"/>
+        <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="rect"/>
       </spPr>
     </pic>
     <clientData/>
@@ -847,17 +847,17 @@
     <ext cx="5715000" cy="3429000"/>
     <pic>
       <nvPicPr>
-        <cNvPr descr="Picture" id="9" name="Image 9"/>
+        <cNvPr id="9" name="Image 9" descr="Picture"/>
         <cNvPicPr/>
       </nvPicPr>
       <blipFill>
-        <a:blip cstate="print" r:embed="rId9"/>
-        <a:stretch>
+        <a:blip xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" cstate="print" r:embed="rId9"/>
+        <a:stretch xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
           <a:fillRect/>
         </a:stretch>
       </blipFill>
       <spPr>
-        <a:prstGeom prst="rect"/>
+        <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="rect"/>
       </spPr>
     </pic>
     <clientData/>
@@ -872,17 +872,17 @@
     <ext cx="5715000" cy="3429000"/>
     <pic>
       <nvPicPr>
-        <cNvPr descr="Picture" id="10" name="Image 10"/>
+        <cNvPr id="10" name="Image 10" descr="Picture"/>
         <cNvPicPr/>
       </nvPicPr>
       <blipFill>
-        <a:blip cstate="print" r:embed="rId10"/>
-        <a:stretch>
+        <a:blip xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" cstate="print" r:embed="rId10"/>
+        <a:stretch xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
           <a:fillRect/>
         </a:stretch>
       </blipFill>
       <spPr>
-        <a:prstGeom prst="rect"/>
+        <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="rect"/>
       </spPr>
     </pic>
     <clientData/>
@@ -897,17 +897,17 @@
     <ext cx="5715000" cy="3429000"/>
     <pic>
       <nvPicPr>
-        <cNvPr descr="Picture" id="11" name="Image 11"/>
+        <cNvPr id="11" name="Image 11" descr="Picture"/>
         <cNvPicPr/>
       </nvPicPr>
       <blipFill>
-        <a:blip cstate="print" r:embed="rId11"/>
-        <a:stretch>
+        <a:blip xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" cstate="print" r:embed="rId11"/>
+        <a:stretch xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
           <a:fillRect/>
         </a:stretch>
       </blipFill>
       <spPr>
-        <a:prstGeom prst="rect"/>
+        <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="rect"/>
       </spPr>
     </pic>
     <clientData/>
@@ -922,17 +922,17 @@
     <ext cx="5715000" cy="3429000"/>
     <pic>
       <nvPicPr>
-        <cNvPr descr="Picture" id="12" name="Image 12"/>
+        <cNvPr id="12" name="Image 12" descr="Picture"/>
         <cNvPicPr/>
       </nvPicPr>
       <blipFill>
-        <a:blip cstate="print" r:embed="rId12"/>
-        <a:stretch>
+        <a:blip xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" cstate="print" r:embed="rId12"/>
+        <a:stretch xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
           <a:fillRect/>
         </a:stretch>
       </blipFill>
       <spPr>
-        <a:prstGeom prst="rect"/>
+        <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="rect"/>
       </spPr>
     </pic>
     <clientData/>
@@ -941,7 +941,7 @@
 </file>
 
 <file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
-<wsDr xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
+<wsDr xmlns="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
   <oneCellAnchor>
     <from>
       <col>0</col>
@@ -952,17 +952,17 @@
     <ext cx="12382500" cy="4953000"/>
     <pic>
       <nvPicPr>
-        <cNvPr descr="Picture" id="1" name="Image 1"/>
+        <cNvPr id="1" name="Image 1" descr="Picture"/>
         <cNvPicPr/>
       </nvPicPr>
       <blipFill>
-        <a:blip cstate="print" r:embed="rId1"/>
-        <a:stretch>
+        <a:blip xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" cstate="print" r:embed="rId1"/>
+        <a:stretch xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
           <a:fillRect/>
         </a:stretch>
       </blipFill>
       <spPr>
-        <a:prstGeom prst="rect"/>
+        <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="rect"/>
       </spPr>
     </pic>
     <clientData/>
@@ -971,7 +971,7 @@
 </file>
 
 <file path=xl/drawings/drawing4.xml><?xml version="1.0" encoding="utf-8"?>
-<wsDr xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
+<wsDr xmlns="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
   <oneCellAnchor>
     <from>
       <col>0</col>
@@ -982,17 +982,17 @@
     <ext cx="12382500" cy="6191250"/>
     <pic>
       <nvPicPr>
-        <cNvPr descr="Picture" id="1" name="Image 1"/>
+        <cNvPr id="1" name="Image 1" descr="Picture"/>
         <cNvPicPr/>
       </nvPicPr>
       <blipFill>
-        <a:blip cstate="print" r:embed="rId1"/>
-        <a:stretch>
+        <a:blip xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" cstate="print" r:embed="rId1"/>
+        <a:stretch xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
           <a:fillRect/>
         </a:stretch>
       </blipFill>
       <spPr>
-        <a:prstGeom prst="rect"/>
+        <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="rect"/>
       </spPr>
     </pic>
     <clientData/>
@@ -1297,8 +1297,8 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <cols>
-    <col customWidth="1" max="1" min="1" width="28"/>
-    <col customWidth="1" max="2" min="2" width="15"/>
+    <col width="28" customWidth="1" min="1" max="1"/>
+    <col width="15" customWidth="1" min="2" max="2"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -1416,12 +1416,12 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
@@ -1434,13 +1434,13 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <cols>
-    <col customWidth="1" max="1" min="1" width="60"/>
-    <col customWidth="1" max="2" min="2" width="15"/>
-    <col customWidth="1" max="3" min="3" width="18"/>
-    <col customWidth="1" max="4" min="4" width="18"/>
-    <col customWidth="1" max="5" min="5" width="18"/>
-    <col customWidth="1" max="6" min="6" width="15"/>
-    <col customWidth="1" max="7" min="7" width="15"/>
+    <col width="60" customWidth="1" min="1" max="1"/>
+    <col width="15" customWidth="1" min="2" max="2"/>
+    <col width="18" customWidth="1" min="3" max="3"/>
+    <col width="18" customWidth="1" min="4" max="4"/>
+    <col width="18" customWidth="1" min="5" max="5"/>
+    <col width="15" customWidth="1" min="6" max="6"/>
+    <col width="15" customWidth="1" min="7" max="7"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -1735,13 +1735,13 @@
     </row>
   </sheetData>
   <autoFilter ref="A1:F3"/>
-  <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
-  <drawing r:id="rId1"/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <drawing xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
@@ -1754,13 +1754,13 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <cols>
-    <col customWidth="1" max="1" min="1" width="60"/>
-    <col customWidth="1" max="2" min="2" width="15"/>
-    <col customWidth="1" max="3" min="3" width="18"/>
-    <col customWidth="1" max="4" min="4" width="18"/>
-    <col customWidth="1" max="5" min="5" width="18"/>
-    <col customWidth="1" max="6" min="6" width="18"/>
-    <col customWidth="1" max="7" min="7" width="15"/>
+    <col width="60" customWidth="1" min="1" max="1"/>
+    <col width="15" customWidth="1" min="2" max="2"/>
+    <col width="18" customWidth="1" min="3" max="3"/>
+    <col width="18" customWidth="1" min="4" max="4"/>
+    <col width="18" customWidth="1" min="5" max="5"/>
+    <col width="18" customWidth="1" min="6" max="6"/>
+    <col width="15" customWidth="1" min="7" max="7"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -2056,7 +2056,7 @@
           <t>1549-9618</t>
         </is>
       </c>
-      <c r="C9" s="11" t="inlineStr">
+      <c r="C9" s="10" t="inlineStr">
         <is>
           <t>B1</t>
         </is>
@@ -2406,7 +2406,7 @@
           <t>0743-7463</t>
         </is>
       </c>
-      <c r="C19" s="11" t="inlineStr">
+      <c r="C19" s="10" t="inlineStr">
         <is>
           <t>B1</t>
         </is>
@@ -2441,7 +2441,7 @@
           <t>1463-9076</t>
         </is>
       </c>
-      <c r="C20" s="11" t="inlineStr">
+      <c r="C20" s="10" t="inlineStr">
         <is>
           <t>B1</t>
         </is>
@@ -2546,7 +2546,7 @@
           <t>1389-2576</t>
         </is>
       </c>
-      <c r="C23" s="11" t="inlineStr">
+      <c r="C23" s="10" t="inlineStr">
         <is>
           <t>B1</t>
         </is>
@@ -2782,8 +2782,8 @@
     </row>
   </sheetData>
   <autoFilter ref="A1:G23"/>
-  <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
-  <drawing r:id="rId1"/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <drawing xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -2801,30 +2801,30 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <cols>
-    <col customWidth="1" max="1" min="1" width="20"/>
-    <col customWidth="1" max="2" min="2" width="15"/>
-    <col customWidth="1" max="3" min="3" width="35"/>
-    <col customWidth="1" max="4" min="4" width="35"/>
-    <col customWidth="1" max="5" min="5" width="20"/>
-    <col customWidth="1" max="6" min="6" width="18"/>
-    <col customWidth="1" max="7" min="7" width="18"/>
-    <col customWidth="1" max="8" min="8" width="18"/>
-    <col customWidth="1" max="9" min="9" width="10"/>
-    <col customWidth="1" max="10" min="10" width="30"/>
-    <col customWidth="1" max="11" min="11" width="30"/>
-    <col customWidth="1" max="12" min="12" width="30"/>
-    <col customWidth="1" max="13" min="13" width="30"/>
-    <col customWidth="1" max="14" min="14" width="30"/>
-    <col customWidth="1" max="15" min="15" width="30"/>
-    <col customWidth="1" max="16" min="16" width="30"/>
-    <col customWidth="1" max="17" min="17" width="30"/>
-    <col customWidth="1" max="18" min="18" width="30"/>
-    <col customWidth="1" max="19" min="19" width="30"/>
-    <col customWidth="1" max="20" min="20" width="30"/>
-    <col customWidth="1" max="21" min="21" width="30"/>
+    <col width="20" customWidth="1" min="1" max="1"/>
+    <col width="15" customWidth="1" min="2" max="2"/>
+    <col width="35" customWidth="1" min="3" max="3"/>
+    <col width="35" customWidth="1" min="4" max="4"/>
+    <col width="20" customWidth="1" min="5" max="5"/>
+    <col width="18" customWidth="1" min="6" max="6"/>
+    <col width="18" customWidth="1" min="7" max="7"/>
+    <col width="18" customWidth="1" min="8" max="8"/>
+    <col width="10" customWidth="1" min="9" max="9"/>
+    <col width="30" customWidth="1" min="10" max="10"/>
+    <col width="30" customWidth="1" min="11" max="11"/>
+    <col width="30" customWidth="1" min="12" max="12"/>
+    <col width="30" customWidth="1" min="13" max="13"/>
+    <col width="30" customWidth="1" min="14" max="14"/>
+    <col width="30" customWidth="1" min="15" max="15"/>
+    <col width="30" customWidth="1" min="16" max="16"/>
+    <col width="30" customWidth="1" min="17" max="17"/>
+    <col width="30" customWidth="1" min="18" max="18"/>
+    <col width="30" customWidth="1" min="19" max="19"/>
+    <col width="30" customWidth="1" min="20" max="20"/>
+    <col width="30" customWidth="1" min="21" max="21"/>
   </cols>
   <sheetData>
-    <row customHeight="1" ht="25" r="1">
+    <row r="1" ht="25" customHeight="1">
       <c r="A1" s="1" t="inlineStr">
         <is>
           <t>Ano</t>
@@ -7827,7 +7827,7 @@
     <mergeCell ref="A34:B34"/>
     <mergeCell ref="A59:B59"/>
   </mergeCells>
-  <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
 
@@ -7845,19 +7845,19 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <cols>
-    <col customWidth="1" max="1" min="1" width="20"/>
-    <col customWidth="1" max="2" min="2" width="15"/>
-    <col customWidth="1" max="3" min="3" width="35"/>
-    <col customWidth="1" max="4" min="4" width="35"/>
-    <col customWidth="1" max="5" min="5" width="20"/>
-    <col customWidth="1" max="6" min="6" width="18"/>
-    <col customWidth="1" max="7" min="7" width="18"/>
-    <col customWidth="1" max="8" min="8" width="18"/>
-    <col customWidth="1" max="9" min="9" width="10"/>
-    <col customWidth="1" max="10" min="10" width="30"/>
+    <col width="20" customWidth="1" min="1" max="1"/>
+    <col width="15" customWidth="1" min="2" max="2"/>
+    <col width="35" customWidth="1" min="3" max="3"/>
+    <col width="35" customWidth="1" min="4" max="4"/>
+    <col width="20" customWidth="1" min="5" max="5"/>
+    <col width="18" customWidth="1" min="6" max="6"/>
+    <col width="18" customWidth="1" min="7" max="7"/>
+    <col width="18" customWidth="1" min="8" max="8"/>
+    <col width="10" customWidth="1" min="9" max="9"/>
+    <col width="30" customWidth="1" min="10" max="10"/>
   </cols>
   <sheetData>
-    <row customHeight="1" ht="25" r="1">
+    <row r="1" ht="25" customHeight="1">
       <c r="A1" s="1" t="inlineStr">
         <is>
           <t>Nome Trabalho</t>
@@ -7876,7 +7876,7 @@
     </row>
   </sheetData>
   <autoFilter ref="A1:C1"/>
-  <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
 
@@ -7894,13 +7894,13 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <cols>
-    <col customWidth="1" max="1" min="1" width="20"/>
-    <col customWidth="1" max="2" min="2" width="15"/>
-    <col customWidth="1" max="3" min="3" width="15"/>
-    <col customWidth="1" max="4" min="4" width="10"/>
-    <col customWidth="1" max="5" min="5" width="20"/>
-    <col customWidth="1" max="6" min="6" width="15"/>
-    <col customWidth="1" max="7" min="7" width="15"/>
+    <col width="20" customWidth="1" min="1" max="1"/>
+    <col width="15" customWidth="1" min="2" max="2"/>
+    <col width="15" customWidth="1" min="3" max="3"/>
+    <col width="10" customWidth="1" min="4" max="4"/>
+    <col width="20" customWidth="1" min="5" max="5"/>
+    <col width="15" customWidth="1" min="6" max="6"/>
+    <col width="15" customWidth="1" min="7" max="7"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -8295,7 +8295,7 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
 
@@ -8313,16 +8313,16 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <cols>
-    <col customWidth="1" max="1" min="1" width="50"/>
-    <col customWidth="1" max="2" min="2" width="10"/>
-    <col customWidth="1" max="3" min="3" width="10"/>
-    <col customWidth="1" max="4" min="4" width="10"/>
-    <col customWidth="1" max="5" min="5" width="10"/>
-    <col customWidth="1" max="6" min="6" width="10"/>
-    <col customWidth="1" max="7" min="7" width="10"/>
+    <col width="50" customWidth="1" min="1" max="1"/>
+    <col width="10" customWidth="1" min="2" max="2"/>
+    <col width="10" customWidth="1" min="3" max="3"/>
+    <col width="10" customWidth="1" min="4" max="4"/>
+    <col width="10" customWidth="1" min="5" max="5"/>
+    <col width="10" customWidth="1" min="6" max="6"/>
+    <col width="10" customWidth="1" min="7" max="7"/>
   </cols>
   <sheetData>
-    <row customHeight="1" ht="25" r="1">
+    <row r="1" ht="25" customHeight="1">
       <c r="A1" s="1" t="inlineStr">
         <is>
           <t>Autor</t>
@@ -10534,7 +10534,7 @@
     </row>
   </sheetData>
   <autoFilter ref="A1:G66"/>
-  <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
 
@@ -10552,28 +10552,28 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <cols>
-    <col customWidth="1" max="1" min="1" width="20"/>
-    <col customWidth="1" max="2" min="2" width="15"/>
-    <col customWidth="1" max="3" min="3" width="35"/>
-    <col customWidth="1" max="4" min="4" width="35"/>
-    <col customWidth="1" max="5" min="5" width="20"/>
-    <col customWidth="1" max="6" min="6" width="18"/>
-    <col customWidth="1" max="7" min="7" width="18"/>
-    <col customWidth="1" max="8" min="8" width="18"/>
-    <col customWidth="1" max="9" min="9" width="18"/>
-    <col customWidth="1" max="10" min="10" width="10"/>
-    <col customWidth="1" max="11" min="11" width="30"/>
-    <col customWidth="1" max="12" min="12" width="30"/>
-    <col customWidth="1" max="13" min="13" width="30"/>
-    <col customWidth="1" max="14" min="14" width="30"/>
-    <col customWidth="1" max="15" min="15" width="30"/>
-    <col customWidth="1" max="16" min="16" width="30"/>
-    <col customWidth="1" max="17" min="17" width="30"/>
-    <col customWidth="1" max="18" min="18" width="30"/>
-    <col customWidth="1" max="19" min="19" width="30"/>
-    <col customWidth="1" max="20" min="20" width="30"/>
-    <col customWidth="1" max="21" min="21" width="30"/>
-    <col customWidth="1" max="22" min="22" width="30"/>
+    <col width="20" customWidth="1" min="1" max="1"/>
+    <col width="15" customWidth="1" min="2" max="2"/>
+    <col width="35" customWidth="1" min="3" max="3"/>
+    <col width="35" customWidth="1" min="4" max="4"/>
+    <col width="20" customWidth="1" min="5" max="5"/>
+    <col width="18" customWidth="1" min="6" max="6"/>
+    <col width="18" customWidth="1" min="7" max="7"/>
+    <col width="18" customWidth="1" min="8" max="8"/>
+    <col width="18" customWidth="1" min="9" max="9"/>
+    <col width="10" customWidth="1" min="10" max="10"/>
+    <col width="30" customWidth="1" min="11" max="11"/>
+    <col width="30" customWidth="1" min="12" max="12"/>
+    <col width="30" customWidth="1" min="13" max="13"/>
+    <col width="30" customWidth="1" min="14" max="14"/>
+    <col width="30" customWidth="1" min="15" max="15"/>
+    <col width="30" customWidth="1" min="16" max="16"/>
+    <col width="30" customWidth="1" min="17" max="17"/>
+    <col width="30" customWidth="1" min="18" max="18"/>
+    <col width="30" customWidth="1" min="19" max="19"/>
+    <col width="30" customWidth="1" min="20" max="20"/>
+    <col width="30" customWidth="1" min="21" max="21"/>
+    <col width="30" customWidth="1" min="22" max="22"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -15494,12 +15494,12 @@
     </row>
   </sheetData>
   <autoFilter ref="A1:V23"/>
-  <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
@@ -15512,16 +15512,16 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <cols>
-    <col customWidth="1" max="1" min="1" width="30"/>
-    <col customWidth="1" max="2" min="2" width="30"/>
-    <col customWidth="1" max="3" min="3" width="30"/>
-    <col customWidth="1" max="4" min="4" width="30"/>
-    <col customWidth="1" max="5" min="5" width="30"/>
-    <col customWidth="1" max="6" min="6" width="30"/>
-    <col customWidth="1" max="7" min="7" width="30"/>
+    <col width="30" customWidth="1" min="1" max="1"/>
+    <col width="30" customWidth="1" min="2" max="2"/>
+    <col width="30" customWidth="1" min="3" max="3"/>
+    <col width="30" customWidth="1" min="4" max="4"/>
+    <col width="30" customWidth="1" min="5" max="5"/>
+    <col width="30" customWidth="1" min="6" max="6"/>
+    <col width="30" customWidth="1" min="7" max="7"/>
   </cols>
   <sheetData>
-    <row customHeight="1" ht="50" r="1">
+    <row r="1" ht="50" customHeight="1">
       <c r="A1" s="5" t="n"/>
       <c r="B1" s="9" t="n"/>
       <c r="C1" s="9" t="n"/>
@@ -15530,7 +15530,7 @@
       <c r="F1" s="9" t="n"/>
       <c r="G1" s="9" t="n"/>
     </row>
-    <row customHeight="1" ht="50" r="2">
+    <row r="2" ht="50" customHeight="1">
       <c r="A2" s="9" t="n"/>
       <c r="B2" s="9" t="n"/>
       <c r="C2" s="9" t="n"/>
@@ -15539,7 +15539,7 @@
       <c r="F2" s="9" t="n"/>
       <c r="G2" s="9" t="n"/>
     </row>
-    <row customHeight="1" ht="50" r="3">
+    <row r="3" ht="50" customHeight="1">
       <c r="A3" s="9" t="n"/>
       <c r="B3" s="9" t="n"/>
       <c r="C3" s="9" t="n"/>
@@ -15548,7 +15548,7 @@
       <c r="F3" s="9" t="n"/>
       <c r="G3" s="9" t="n"/>
     </row>
-    <row customHeight="1" ht="50" r="4">
+    <row r="4" ht="50" customHeight="1">
       <c r="A4" s="9" t="n"/>
       <c r="B4" s="9" t="n"/>
       <c r="C4" s="9" t="n"/>
@@ -15557,7 +15557,7 @@
       <c r="F4" s="9" t="n"/>
       <c r="G4" s="9" t="n"/>
     </row>
-    <row customHeight="1" ht="50" r="5">
+    <row r="5" ht="50" customHeight="1">
       <c r="A5" s="9" t="n"/>
       <c r="B5" s="9" t="n"/>
       <c r="C5" s="9" t="n"/>
@@ -15566,7 +15566,7 @@
       <c r="F5" s="9" t="n"/>
       <c r="G5" s="9" t="n"/>
     </row>
-    <row customHeight="1" ht="50" r="6">
+    <row r="6" ht="50" customHeight="1">
       <c r="A6" s="9" t="n"/>
       <c r="B6" s="9" t="n"/>
       <c r="C6" s="9" t="n"/>
@@ -15575,7 +15575,7 @@
       <c r="F6" s="9" t="n"/>
       <c r="G6" s="9" t="n"/>
     </row>
-    <row customHeight="1" ht="50" r="7">
+    <row r="7" ht="50" customHeight="1">
       <c r="A7" s="9" t="n"/>
       <c r="B7" s="9" t="n"/>
       <c r="C7" s="9" t="n"/>
@@ -15584,7 +15584,7 @@
       <c r="F7" s="9" t="n"/>
       <c r="G7" s="9" t="n"/>
     </row>
-    <row customHeight="1" ht="50" r="8">
+    <row r="8" ht="50" customHeight="1">
       <c r="A8" s="9" t="n"/>
       <c r="B8" s="9" t="n"/>
       <c r="C8" s="9" t="n"/>
@@ -15593,7 +15593,7 @@
       <c r="F8" s="9" t="n"/>
       <c r="G8" s="9" t="n"/>
     </row>
-    <row customHeight="1" ht="50" r="9">
+    <row r="9" ht="50" customHeight="1">
       <c r="A9" s="9" t="n"/>
       <c r="B9" s="9" t="n"/>
       <c r="C9" s="9" t="n"/>
@@ -15602,7 +15602,7 @@
       <c r="F9" s="9" t="n"/>
       <c r="G9" s="9" t="n"/>
     </row>
-    <row customHeight="1" ht="50" r="10">
+    <row r="10" ht="50" customHeight="1">
       <c r="A10" s="9" t="n"/>
       <c r="B10" s="9" t="n"/>
       <c r="C10" s="9" t="n"/>
@@ -15611,7 +15611,7 @@
       <c r="F10" s="9" t="n"/>
       <c r="G10" s="9" t="n"/>
     </row>
-    <row customHeight="1" ht="50" r="11">
+    <row r="11" ht="50" customHeight="1">
       <c r="A11" s="9" t="n"/>
       <c r="B11" s="9" t="n"/>
       <c r="C11" s="9" t="n"/>
@@ -15620,7 +15620,7 @@
       <c r="F11" s="9" t="n"/>
       <c r="G11" s="9" t="n"/>
     </row>
-    <row customHeight="1" ht="50" r="12">
+    <row r="12" ht="50" customHeight="1">
       <c r="A12" s="9" t="n"/>
       <c r="B12" s="9" t="n"/>
       <c r="C12" s="9" t="n"/>
@@ -15629,7 +15629,7 @@
       <c r="F12" s="9" t="n"/>
       <c r="G12" s="9" t="n"/>
     </row>
-    <row customHeight="1" ht="50" r="13">
+    <row r="13" ht="50" customHeight="1">
       <c r="A13" s="9" t="n"/>
       <c r="B13" s="9" t="n"/>
       <c r="C13" s="9" t="n"/>
@@ -15638,7 +15638,7 @@
       <c r="F13" s="9" t="n"/>
       <c r="G13" s="9" t="n"/>
     </row>
-    <row customHeight="1" ht="50" r="14">
+    <row r="14" ht="50" customHeight="1">
       <c r="A14" s="9" t="n"/>
       <c r="B14" s="9" t="n"/>
       <c r="C14" s="9" t="n"/>
@@ -15647,7 +15647,7 @@
       <c r="F14" s="9" t="n"/>
       <c r="G14" s="9" t="n"/>
     </row>
-    <row customHeight="1" ht="50" r="15">
+    <row r="15" ht="50" customHeight="1">
       <c r="A15" s="9" t="n"/>
       <c r="B15" s="9" t="n"/>
       <c r="C15" s="9" t="n"/>
@@ -15656,7 +15656,7 @@
       <c r="F15" s="9" t="n"/>
       <c r="G15" s="9" t="n"/>
     </row>
-    <row customHeight="1" ht="50" r="16">
+    <row r="16" ht="50" customHeight="1">
       <c r="A16" s="9" t="n"/>
       <c r="B16" s="9" t="n"/>
       <c r="C16" s="9" t="n"/>
@@ -15665,7 +15665,7 @@
       <c r="F16" s="9" t="n"/>
       <c r="G16" s="9" t="n"/>
     </row>
-    <row customHeight="1" ht="50" r="17">
+    <row r="17" ht="50" customHeight="1">
       <c r="A17" s="9" t="n"/>
       <c r="B17" s="9" t="n"/>
       <c r="C17" s="9" t="n"/>
@@ -15674,7 +15674,7 @@
       <c r="F17" s="9" t="n"/>
       <c r="G17" s="9" t="n"/>
     </row>
-    <row customHeight="1" ht="50" r="18">
+    <row r="18" ht="50" customHeight="1">
       <c r="A18" s="9" t="n"/>
       <c r="B18" s="9" t="n"/>
       <c r="C18" s="9" t="n"/>
@@ -15683,7 +15683,7 @@
       <c r="F18" s="9" t="n"/>
       <c r="G18" s="9" t="n"/>
     </row>
-    <row customHeight="1" ht="50" r="19">
+    <row r="19" ht="50" customHeight="1">
       <c r="A19" s="9" t="n"/>
       <c r="B19" s="9" t="n"/>
       <c r="C19" s="9" t="n"/>
@@ -15692,7 +15692,7 @@
       <c r="F19" s="9" t="n"/>
       <c r="G19" s="9" t="n"/>
     </row>
-    <row customHeight="1" ht="50" r="20">
+    <row r="20" ht="50" customHeight="1">
       <c r="A20" s="9" t="n"/>
       <c r="B20" s="9" t="n"/>
       <c r="C20" s="9" t="n"/>
@@ -15701,7 +15701,7 @@
       <c r="F20" s="9" t="n"/>
       <c r="G20" s="9" t="n"/>
     </row>
-    <row customHeight="1" ht="50" r="21">
+    <row r="21" ht="50" customHeight="1">
       <c r="A21" s="9" t="n"/>
       <c r="B21" s="9" t="n"/>
       <c r="C21" s="9" t="n"/>
@@ -15710,7 +15710,7 @@
       <c r="F21" s="9" t="n"/>
       <c r="G21" s="9" t="n"/>
     </row>
-    <row customHeight="1" ht="50" r="22">
+    <row r="22" ht="50" customHeight="1">
       <c r="A22" s="9" t="n"/>
       <c r="B22" s="9" t="n"/>
       <c r="C22" s="9" t="n"/>
@@ -15719,7 +15719,7 @@
       <c r="F22" s="9" t="n"/>
       <c r="G22" s="9" t="n"/>
     </row>
-    <row customHeight="1" ht="50" r="23">
+    <row r="23" ht="50" customHeight="1">
       <c r="A23" s="9" t="n"/>
       <c r="B23" s="9" t="n"/>
       <c r="C23" s="9" t="n"/>
@@ -15728,7 +15728,7 @@
       <c r="F23" s="9" t="n"/>
       <c r="G23" s="9" t="n"/>
     </row>
-    <row customHeight="1" ht="50" r="24">
+    <row r="24" ht="50" customHeight="1">
       <c r="A24" s="9" t="n"/>
       <c r="B24" s="9" t="n"/>
       <c r="C24" s="9" t="n"/>
@@ -15737,7 +15737,7 @@
       <c r="F24" s="9" t="n"/>
       <c r="G24" s="9" t="n"/>
     </row>
-    <row customHeight="1" ht="50" r="25">
+    <row r="25" ht="50" customHeight="1">
       <c r="A25" s="9" t="n"/>
       <c r="B25" s="9" t="n"/>
       <c r="C25" s="9" t="n"/>
@@ -15746,7 +15746,7 @@
       <c r="F25" s="9" t="n"/>
       <c r="G25" s="9" t="n"/>
     </row>
-    <row customHeight="1" ht="50" r="26">
+    <row r="26" ht="50" customHeight="1">
       <c r="A26" s="9" t="n"/>
       <c r="B26" s="9" t="n"/>
       <c r="C26" s="9" t="n"/>
@@ -15755,7 +15755,7 @@
       <c r="F26" s="9" t="n"/>
       <c r="G26" s="9" t="n"/>
     </row>
-    <row customHeight="1" ht="50" r="27">
+    <row r="27" ht="50" customHeight="1">
       <c r="A27" s="9" t="n"/>
       <c r="B27" s="9" t="n"/>
       <c r="C27" s="9" t="n"/>
@@ -15764,7 +15764,7 @@
       <c r="F27" s="9" t="n"/>
       <c r="G27" s="9" t="n"/>
     </row>
-    <row customHeight="1" ht="50" r="28">
+    <row r="28" ht="50" customHeight="1">
       <c r="A28" s="9" t="n"/>
       <c r="B28" s="9" t="n"/>
       <c r="C28" s="9" t="n"/>
@@ -15773,7 +15773,7 @@
       <c r="F28" s="9" t="n"/>
       <c r="G28" s="9" t="n"/>
     </row>
-    <row customHeight="1" ht="50" r="29">
+    <row r="29" ht="50" customHeight="1">
       <c r="A29" s="9" t="n"/>
       <c r="B29" s="9" t="n"/>
       <c r="C29" s="9" t="n"/>
@@ -15782,7 +15782,7 @@
       <c r="F29" s="9" t="n"/>
       <c r="G29" s="9" t="n"/>
     </row>
-    <row customHeight="1" ht="50" r="30">
+    <row r="30" ht="50" customHeight="1">
       <c r="A30" s="9" t="n"/>
       <c r="B30" s="9" t="n"/>
       <c r="C30" s="9" t="n"/>
@@ -15791,7 +15791,7 @@
       <c r="F30" s="9" t="n"/>
       <c r="G30" s="9" t="n"/>
     </row>
-    <row customHeight="1" ht="50" r="31">
+    <row r="31" ht="50" customHeight="1">
       <c r="A31" s="9" t="n"/>
       <c r="B31" s="9" t="n"/>
       <c r="C31" s="9" t="n"/>
@@ -15800,7 +15800,7 @@
       <c r="F31" s="9" t="n"/>
       <c r="G31" s="9" t="n"/>
     </row>
-    <row customHeight="1" ht="50" r="32">
+    <row r="32" ht="50" customHeight="1">
       <c r="A32" s="9" t="n"/>
       <c r="B32" s="9" t="n"/>
       <c r="C32" s="9" t="n"/>
@@ -15809,7 +15809,7 @@
       <c r="F32" s="9" t="n"/>
       <c r="G32" s="9" t="n"/>
     </row>
-    <row customHeight="1" ht="50" r="33">
+    <row r="33" ht="50" customHeight="1">
       <c r="A33" s="9" t="n"/>
       <c r="B33" s="9" t="n"/>
       <c r="C33" s="9" t="n"/>
@@ -15818,7 +15818,7 @@
       <c r="F33" s="9" t="n"/>
       <c r="G33" s="9" t="n"/>
     </row>
-    <row customHeight="1" ht="50" r="34">
+    <row r="34" ht="50" customHeight="1">
       <c r="A34" s="9" t="n"/>
       <c r="B34" s="9" t="n"/>
       <c r="C34" s="9" t="n"/>
@@ -15827,7 +15827,7 @@
       <c r="F34" s="9" t="n"/>
       <c r="G34" s="9" t="n"/>
     </row>
-    <row customHeight="1" ht="50" r="35">
+    <row r="35" ht="50" customHeight="1">
       <c r="A35" s="9" t="n"/>
       <c r="B35" s="9" t="n"/>
       <c r="C35" s="9" t="n"/>
@@ -15836,7 +15836,7 @@
       <c r="F35" s="9" t="n"/>
       <c r="G35" s="9" t="n"/>
     </row>
-    <row customHeight="1" ht="50" r="36">
+    <row r="36" ht="50" customHeight="1">
       <c r="A36" s="9" t="n"/>
       <c r="B36" s="9" t="n"/>
       <c r="C36" s="9" t="n"/>
@@ -15845,7 +15845,7 @@
       <c r="F36" s="9" t="n"/>
       <c r="G36" s="9" t="n"/>
     </row>
-    <row customHeight="1" ht="50" r="37">
+    <row r="37" ht="50" customHeight="1">
       <c r="A37" s="9" t="n"/>
       <c r="B37" s="9" t="n"/>
       <c r="C37" s="9" t="n"/>
@@ -15854,7 +15854,7 @@
       <c r="F37" s="9" t="n"/>
       <c r="G37" s="9" t="n"/>
     </row>
-    <row customHeight="1" ht="50" r="38">
+    <row r="38" ht="50" customHeight="1">
       <c r="A38" s="9" t="n"/>
       <c r="B38" s="9" t="n"/>
       <c r="C38" s="9" t="n"/>
@@ -15863,7 +15863,7 @@
       <c r="F38" s="9" t="n"/>
       <c r="G38" s="9" t="n"/>
     </row>
-    <row customHeight="1" ht="50" r="39">
+    <row r="39" ht="50" customHeight="1">
       <c r="A39" s="9" t="n"/>
       <c r="B39" s="9" t="n"/>
       <c r="C39" s="9" t="n"/>
@@ -15872,7 +15872,7 @@
       <c r="F39" s="9" t="n"/>
       <c r="G39" s="9" t="n"/>
     </row>
-    <row customHeight="1" ht="50" r="40">
+    <row r="40" ht="50" customHeight="1">
       <c r="A40" s="9" t="n"/>
       <c r="B40" s="9" t="n"/>
       <c r="C40" s="9" t="n"/>
@@ -15881,7 +15881,7 @@
       <c r="F40" s="9" t="n"/>
       <c r="G40" s="9" t="n"/>
     </row>
-    <row customHeight="1" ht="50" r="41">
+    <row r="41" ht="50" customHeight="1">
       <c r="A41" s="9" t="n"/>
       <c r="B41" s="9" t="n"/>
       <c r="C41" s="9" t="n"/>
@@ -15890,7 +15890,7 @@
       <c r="F41" s="9" t="n"/>
       <c r="G41" s="9" t="n"/>
     </row>
-    <row customHeight="1" ht="50" r="42">
+    <row r="42" ht="50" customHeight="1">
       <c r="A42" s="9" t="n"/>
       <c r="B42" s="9" t="n"/>
       <c r="C42" s="9" t="n"/>
@@ -15899,7 +15899,7 @@
       <c r="F42" s="9" t="n"/>
       <c r="G42" s="9" t="n"/>
     </row>
-    <row customHeight="1" ht="50" r="43">
+    <row r="43" ht="50" customHeight="1">
       <c r="A43" s="9" t="n"/>
       <c r="B43" s="9" t="n"/>
       <c r="C43" s="9" t="n"/>
@@ -15908,7 +15908,7 @@
       <c r="F43" s="9" t="n"/>
       <c r="G43" s="9" t="n"/>
     </row>
-    <row customHeight="1" ht="50" r="44">
+    <row r="44" ht="50" customHeight="1">
       <c r="A44" s="9" t="n"/>
       <c r="B44" s="9" t="n"/>
       <c r="C44" s="9" t="n"/>
@@ -15917,7 +15917,7 @@
       <c r="F44" s="9" t="n"/>
       <c r="G44" s="9" t="n"/>
     </row>
-    <row customHeight="1" ht="50" r="45">
+    <row r="45" ht="50" customHeight="1">
       <c r="A45" s="9" t="n"/>
       <c r="B45" s="9" t="n"/>
       <c r="C45" s="9" t="n"/>
@@ -15926,7 +15926,7 @@
       <c r="F45" s="9" t="n"/>
       <c r="G45" s="9" t="n"/>
     </row>
-    <row customHeight="1" ht="50" r="46">
+    <row r="46" ht="50" customHeight="1">
       <c r="A46" s="9" t="n"/>
       <c r="B46" s="9" t="n"/>
       <c r="C46" s="9" t="n"/>
@@ -15935,7 +15935,7 @@
       <c r="F46" s="9" t="n"/>
       <c r="G46" s="9" t="n"/>
     </row>
-    <row customHeight="1" ht="50" r="47">
+    <row r="47" ht="50" customHeight="1">
       <c r="A47" s="9" t="n"/>
       <c r="B47" s="9" t="n"/>
       <c r="C47" s="9" t="n"/>
@@ -15944,7 +15944,7 @@
       <c r="F47" s="9" t="n"/>
       <c r="G47" s="9" t="n"/>
     </row>
-    <row customHeight="1" ht="50" r="48">
+    <row r="48" ht="50" customHeight="1">
       <c r="A48" s="9" t="n"/>
       <c r="B48" s="9" t="n"/>
       <c r="C48" s="9" t="n"/>
@@ -15953,7 +15953,7 @@
       <c r="F48" s="9" t="n"/>
       <c r="G48" s="9" t="n"/>
     </row>
-    <row customHeight="1" ht="50" r="49">
+    <row r="49" ht="50" customHeight="1">
       <c r="A49" s="9" t="n"/>
       <c r="B49" s="9" t="n"/>
       <c r="C49" s="9" t="n"/>
@@ -15962,7 +15962,7 @@
       <c r="F49" s="9" t="n"/>
       <c r="G49" s="9" t="n"/>
     </row>
-    <row customHeight="1" ht="50" r="50">
+    <row r="50" ht="50" customHeight="1">
       <c r="A50" s="9" t="n"/>
       <c r="B50" s="9" t="n"/>
       <c r="C50" s="9" t="n"/>
@@ -15972,13 +15972,13 @@
       <c r="G50" s="9" t="n"/>
     </row>
   </sheetData>
-  <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
-  <drawing r:id="rId1"/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <drawing xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
@@ -15991,16 +15991,16 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <cols>
-    <col customWidth="1" max="1" min="1" width="30"/>
-    <col customWidth="1" max="2" min="2" width="30"/>
-    <col customWidth="1" max="3" min="3" width="30"/>
-    <col customWidth="1" max="4" min="4" width="30"/>
-    <col customWidth="1" max="5" min="5" width="30"/>
-    <col customWidth="1" max="6" min="6" width="30"/>
-    <col customWidth="1" max="7" min="7" width="30"/>
+    <col width="30" customWidth="1" min="1" max="1"/>
+    <col width="30" customWidth="1" min="2" max="2"/>
+    <col width="30" customWidth="1" min="3" max="3"/>
+    <col width="30" customWidth="1" min="4" max="4"/>
+    <col width="30" customWidth="1" min="5" max="5"/>
+    <col width="30" customWidth="1" min="6" max="6"/>
+    <col width="30" customWidth="1" min="7" max="7"/>
   </cols>
   <sheetData>
-    <row customHeight="1" ht="50" r="1">
+    <row r="1" ht="50" customHeight="1">
       <c r="A1" s="5" t="n"/>
       <c r="B1" s="9" t="n"/>
       <c r="C1" s="9" t="n"/>
@@ -16009,7 +16009,7 @@
       <c r="F1" s="9" t="n"/>
       <c r="G1" s="9" t="n"/>
     </row>
-    <row customHeight="1" ht="50" r="2">
+    <row r="2" ht="50" customHeight="1">
       <c r="A2" s="9" t="n"/>
       <c r="B2" s="9" t="n"/>
       <c r="C2" s="9" t="n"/>
@@ -16018,7 +16018,7 @@
       <c r="F2" s="9" t="n"/>
       <c r="G2" s="9" t="n"/>
     </row>
-    <row customHeight="1" ht="50" r="3">
+    <row r="3" ht="50" customHeight="1">
       <c r="A3" s="9" t="n"/>
       <c r="B3" s="9" t="n"/>
       <c r="C3" s="9" t="n"/>
@@ -16027,7 +16027,7 @@
       <c r="F3" s="9" t="n"/>
       <c r="G3" s="9" t="n"/>
     </row>
-    <row customHeight="1" ht="50" r="4">
+    <row r="4" ht="50" customHeight="1">
       <c r="A4" s="9" t="n"/>
       <c r="B4" s="9" t="n"/>
       <c r="C4" s="9" t="n"/>
@@ -16036,7 +16036,7 @@
       <c r="F4" s="9" t="n"/>
       <c r="G4" s="9" t="n"/>
     </row>
-    <row customHeight="1" ht="50" r="5">
+    <row r="5" ht="50" customHeight="1">
       <c r="A5" s="9" t="n"/>
       <c r="B5" s="9" t="n"/>
       <c r="C5" s="9" t="n"/>
@@ -16045,7 +16045,7 @@
       <c r="F5" s="9" t="n"/>
       <c r="G5" s="9" t="n"/>
     </row>
-    <row customHeight="1" ht="50" r="6">
+    <row r="6" ht="50" customHeight="1">
       <c r="A6" s="9" t="n"/>
       <c r="B6" s="9" t="n"/>
       <c r="C6" s="9" t="n"/>
@@ -16054,7 +16054,7 @@
       <c r="F6" s="9" t="n"/>
       <c r="G6" s="9" t="n"/>
     </row>
-    <row customHeight="1" ht="50" r="7">
+    <row r="7" ht="50" customHeight="1">
       <c r="A7" s="9" t="n"/>
       <c r="B7" s="9" t="n"/>
       <c r="C7" s="9" t="n"/>
@@ -16063,7 +16063,7 @@
       <c r="F7" s="9" t="n"/>
       <c r="G7" s="9" t="n"/>
     </row>
-    <row customHeight="1" ht="50" r="8">
+    <row r="8" ht="50" customHeight="1">
       <c r="A8" s="9" t="n"/>
       <c r="B8" s="9" t="n"/>
       <c r="C8" s="9" t="n"/>
@@ -16072,7 +16072,7 @@
       <c r="F8" s="9" t="n"/>
       <c r="G8" s="9" t="n"/>
     </row>
-    <row customHeight="1" ht="50" r="9">
+    <row r="9" ht="50" customHeight="1">
       <c r="A9" s="9" t="n"/>
       <c r="B9" s="9" t="n"/>
       <c r="C9" s="9" t="n"/>
@@ -16081,7 +16081,7 @@
       <c r="F9" s="9" t="n"/>
       <c r="G9" s="9" t="n"/>
     </row>
-    <row customHeight="1" ht="50" r="10">
+    <row r="10" ht="50" customHeight="1">
       <c r="A10" s="9" t="n"/>
       <c r="B10" s="9" t="n"/>
       <c r="C10" s="9" t="n"/>
@@ -16090,7 +16090,7 @@
       <c r="F10" s="9" t="n"/>
       <c r="G10" s="9" t="n"/>
     </row>
-    <row customHeight="1" ht="50" r="11">
+    <row r="11" ht="50" customHeight="1">
       <c r="A11" s="9" t="n"/>
       <c r="B11" s="9" t="n"/>
       <c r="C11" s="9" t="n"/>
@@ -16099,7 +16099,7 @@
       <c r="F11" s="9" t="n"/>
       <c r="G11" s="9" t="n"/>
     </row>
-    <row customHeight="1" ht="50" r="12">
+    <row r="12" ht="50" customHeight="1">
       <c r="A12" s="9" t="n"/>
       <c r="B12" s="9" t="n"/>
       <c r="C12" s="9" t="n"/>
@@ -16108,7 +16108,7 @@
       <c r="F12" s="9" t="n"/>
       <c r="G12" s="9" t="n"/>
     </row>
-    <row customHeight="1" ht="50" r="13">
+    <row r="13" ht="50" customHeight="1">
       <c r="A13" s="9" t="n"/>
       <c r="B13" s="9" t="n"/>
       <c r="C13" s="9" t="n"/>
@@ -16117,7 +16117,7 @@
       <c r="F13" s="9" t="n"/>
       <c r="G13" s="9" t="n"/>
     </row>
-    <row customHeight="1" ht="50" r="14">
+    <row r="14" ht="50" customHeight="1">
       <c r="A14" s="9" t="n"/>
       <c r="B14" s="9" t="n"/>
       <c r="C14" s="9" t="n"/>
@@ -16126,7 +16126,7 @@
       <c r="F14" s="9" t="n"/>
       <c r="G14" s="9" t="n"/>
     </row>
-    <row customHeight="1" ht="50" r="15">
+    <row r="15" ht="50" customHeight="1">
       <c r="A15" s="9" t="n"/>
       <c r="B15" s="9" t="n"/>
       <c r="C15" s="9" t="n"/>
@@ -16135,7 +16135,7 @@
       <c r="F15" s="9" t="n"/>
       <c r="G15" s="9" t="n"/>
     </row>
-    <row customHeight="1" ht="50" r="16">
+    <row r="16" ht="50" customHeight="1">
       <c r="A16" s="9" t="n"/>
       <c r="B16" s="9" t="n"/>
       <c r="C16" s="9" t="n"/>
@@ -16144,7 +16144,7 @@
       <c r="F16" s="9" t="n"/>
       <c r="G16" s="9" t="n"/>
     </row>
-    <row customHeight="1" ht="50" r="17">
+    <row r="17" ht="50" customHeight="1">
       <c r="A17" s="9" t="n"/>
       <c r="B17" s="9" t="n"/>
       <c r="C17" s="9" t="n"/>
@@ -16153,7 +16153,7 @@
       <c r="F17" s="9" t="n"/>
       <c r="G17" s="9" t="n"/>
     </row>
-    <row customHeight="1" ht="50" r="18">
+    <row r="18" ht="50" customHeight="1">
       <c r="A18" s="9" t="n"/>
       <c r="B18" s="9" t="n"/>
       <c r="C18" s="9" t="n"/>
@@ -16162,7 +16162,7 @@
       <c r="F18" s="9" t="n"/>
       <c r="G18" s="9" t="n"/>
     </row>
-    <row customHeight="1" ht="50" r="19">
+    <row r="19" ht="50" customHeight="1">
       <c r="A19" s="9" t="n"/>
       <c r="B19" s="9" t="n"/>
       <c r="C19" s="9" t="n"/>
@@ -16171,7 +16171,7 @@
       <c r="F19" s="9" t="n"/>
       <c r="G19" s="9" t="n"/>
     </row>
-    <row customHeight="1" ht="50" r="20">
+    <row r="20" ht="50" customHeight="1">
       <c r="A20" s="9" t="n"/>
       <c r="B20" s="9" t="n"/>
       <c r="C20" s="9" t="n"/>
@@ -16180,7 +16180,7 @@
       <c r="F20" s="9" t="n"/>
       <c r="G20" s="9" t="n"/>
     </row>
-    <row customHeight="1" ht="50" r="21">
+    <row r="21" ht="50" customHeight="1">
       <c r="A21" s="9" t="n"/>
       <c r="B21" s="9" t="n"/>
       <c r="C21" s="9" t="n"/>
@@ -16189,7 +16189,7 @@
       <c r="F21" s="9" t="n"/>
       <c r="G21" s="9" t="n"/>
     </row>
-    <row customHeight="1" ht="50" r="22">
+    <row r="22" ht="50" customHeight="1">
       <c r="A22" s="9" t="n"/>
       <c r="B22" s="9" t="n"/>
       <c r="C22" s="9" t="n"/>
@@ -16198,7 +16198,7 @@
       <c r="F22" s="9" t="n"/>
       <c r="G22" s="9" t="n"/>
     </row>
-    <row customHeight="1" ht="50" r="23">
+    <row r="23" ht="50" customHeight="1">
       <c r="A23" s="9" t="n"/>
       <c r="B23" s="9" t="n"/>
       <c r="C23" s="9" t="n"/>
@@ -16207,7 +16207,7 @@
       <c r="F23" s="9" t="n"/>
       <c r="G23" s="9" t="n"/>
     </row>
-    <row customHeight="1" ht="50" r="24">
+    <row r="24" ht="50" customHeight="1">
       <c r="A24" s="9" t="n"/>
       <c r="B24" s="9" t="n"/>
       <c r="C24" s="9" t="n"/>
@@ -16216,7 +16216,7 @@
       <c r="F24" s="9" t="n"/>
       <c r="G24" s="9" t="n"/>
     </row>
-    <row customHeight="1" ht="50" r="25">
+    <row r="25" ht="50" customHeight="1">
       <c r="A25" s="9" t="n"/>
       <c r="B25" s="9" t="n"/>
       <c r="C25" s="9" t="n"/>
@@ -16225,7 +16225,7 @@
       <c r="F25" s="9" t="n"/>
       <c r="G25" s="9" t="n"/>
     </row>
-    <row customHeight="1" ht="50" r="26">
+    <row r="26" ht="50" customHeight="1">
       <c r="A26" s="9" t="n"/>
       <c r="B26" s="9" t="n"/>
       <c r="C26" s="9" t="n"/>
@@ -16234,7 +16234,7 @@
       <c r="F26" s="9" t="n"/>
       <c r="G26" s="9" t="n"/>
     </row>
-    <row customHeight="1" ht="50" r="27">
+    <row r="27" ht="50" customHeight="1">
       <c r="A27" s="9" t="n"/>
       <c r="B27" s="9" t="n"/>
       <c r="C27" s="9" t="n"/>
@@ -16243,7 +16243,7 @@
       <c r="F27" s="9" t="n"/>
       <c r="G27" s="9" t="n"/>
     </row>
-    <row customHeight="1" ht="50" r="28">
+    <row r="28" ht="50" customHeight="1">
       <c r="A28" s="9" t="n"/>
       <c r="B28" s="9" t="n"/>
       <c r="C28" s="9" t="n"/>
@@ -16252,7 +16252,7 @@
       <c r="F28" s="9" t="n"/>
       <c r="G28" s="9" t="n"/>
     </row>
-    <row customHeight="1" ht="50" r="29">
+    <row r="29" ht="50" customHeight="1">
       <c r="A29" s="9" t="n"/>
       <c r="B29" s="9" t="n"/>
       <c r="C29" s="9" t="n"/>
@@ -16261,7 +16261,7 @@
       <c r="F29" s="9" t="n"/>
       <c r="G29" s="9" t="n"/>
     </row>
-    <row customHeight="1" ht="50" r="30">
+    <row r="30" ht="50" customHeight="1">
       <c r="A30" s="9" t="n"/>
       <c r="B30" s="9" t="n"/>
       <c r="C30" s="9" t="n"/>
@@ -16270,7 +16270,7 @@
       <c r="F30" s="9" t="n"/>
       <c r="G30" s="9" t="n"/>
     </row>
-    <row customHeight="1" ht="50" r="31">
+    <row r="31" ht="50" customHeight="1">
       <c r="A31" s="9" t="n"/>
       <c r="B31" s="9" t="n"/>
       <c r="C31" s="9" t="n"/>
@@ -16279,7 +16279,7 @@
       <c r="F31" s="9" t="n"/>
       <c r="G31" s="9" t="n"/>
     </row>
-    <row customHeight="1" ht="50" r="32">
+    <row r="32" ht="50" customHeight="1">
       <c r="A32" s="9" t="n"/>
       <c r="B32" s="9" t="n"/>
       <c r="C32" s="9" t="n"/>
@@ -16288,7 +16288,7 @@
       <c r="F32" s="9" t="n"/>
       <c r="G32" s="9" t="n"/>
     </row>
-    <row customHeight="1" ht="50" r="33">
+    <row r="33" ht="50" customHeight="1">
       <c r="A33" s="9" t="n"/>
       <c r="B33" s="9" t="n"/>
       <c r="C33" s="9" t="n"/>
@@ -16297,7 +16297,7 @@
       <c r="F33" s="9" t="n"/>
       <c r="G33" s="9" t="n"/>
     </row>
-    <row customHeight="1" ht="50" r="34">
+    <row r="34" ht="50" customHeight="1">
       <c r="A34" s="9" t="n"/>
       <c r="B34" s="9" t="n"/>
       <c r="C34" s="9" t="n"/>
@@ -16306,7 +16306,7 @@
       <c r="F34" s="9" t="n"/>
       <c r="G34" s="9" t="n"/>
     </row>
-    <row customHeight="1" ht="50" r="35">
+    <row r="35" ht="50" customHeight="1">
       <c r="A35" s="9" t="n"/>
       <c r="B35" s="9" t="n"/>
       <c r="C35" s="9" t="n"/>
@@ -16315,7 +16315,7 @@
       <c r="F35" s="9" t="n"/>
       <c r="G35" s="9" t="n"/>
     </row>
-    <row customHeight="1" ht="50" r="36">
+    <row r="36" ht="50" customHeight="1">
       <c r="A36" s="9" t="n"/>
       <c r="B36" s="9" t="n"/>
       <c r="C36" s="9" t="n"/>
@@ -16324,7 +16324,7 @@
       <c r="F36" s="9" t="n"/>
       <c r="G36" s="9" t="n"/>
     </row>
-    <row customHeight="1" ht="50" r="37">
+    <row r="37" ht="50" customHeight="1">
       <c r="A37" s="9" t="n"/>
       <c r="B37" s="9" t="n"/>
       <c r="C37" s="9" t="n"/>
@@ -16333,7 +16333,7 @@
       <c r="F37" s="9" t="n"/>
       <c r="G37" s="9" t="n"/>
     </row>
-    <row customHeight="1" ht="50" r="38">
+    <row r="38" ht="50" customHeight="1">
       <c r="A38" s="9" t="n"/>
       <c r="B38" s="9" t="n"/>
       <c r="C38" s="9" t="n"/>
@@ -16342,7 +16342,7 @@
       <c r="F38" s="9" t="n"/>
       <c r="G38" s="9" t="n"/>
     </row>
-    <row customHeight="1" ht="50" r="39">
+    <row r="39" ht="50" customHeight="1">
       <c r="A39" s="9" t="n"/>
       <c r="B39" s="9" t="n"/>
       <c r="C39" s="9" t="n"/>
@@ -16351,7 +16351,7 @@
       <c r="F39" s="9" t="n"/>
       <c r="G39" s="9" t="n"/>
     </row>
-    <row customHeight="1" ht="50" r="40">
+    <row r="40" ht="50" customHeight="1">
       <c r="A40" s="9" t="n"/>
       <c r="B40" s="9" t="n"/>
       <c r="C40" s="9" t="n"/>
@@ -16360,7 +16360,7 @@
       <c r="F40" s="9" t="n"/>
       <c r="G40" s="9" t="n"/>
     </row>
-    <row customHeight="1" ht="50" r="41">
+    <row r="41" ht="50" customHeight="1">
       <c r="A41" s="9" t="n"/>
       <c r="B41" s="9" t="n"/>
       <c r="C41" s="9" t="n"/>
@@ -16369,7 +16369,7 @@
       <c r="F41" s="9" t="n"/>
       <c r="G41" s="9" t="n"/>
     </row>
-    <row customHeight="1" ht="50" r="42">
+    <row r="42" ht="50" customHeight="1">
       <c r="A42" s="9" t="n"/>
       <c r="B42" s="9" t="n"/>
       <c r="C42" s="9" t="n"/>
@@ -16378,7 +16378,7 @@
       <c r="F42" s="9" t="n"/>
       <c r="G42" s="9" t="n"/>
     </row>
-    <row customHeight="1" ht="50" r="43">
+    <row r="43" ht="50" customHeight="1">
       <c r="A43" s="9" t="n"/>
       <c r="B43" s="9" t="n"/>
       <c r="C43" s="9" t="n"/>
@@ -16387,7 +16387,7 @@
       <c r="F43" s="9" t="n"/>
       <c r="G43" s="9" t="n"/>
     </row>
-    <row customHeight="1" ht="50" r="44">
+    <row r="44" ht="50" customHeight="1">
       <c r="A44" s="9" t="n"/>
       <c r="B44" s="9" t="n"/>
       <c r="C44" s="9" t="n"/>
@@ -16396,7 +16396,7 @@
       <c r="F44" s="9" t="n"/>
       <c r="G44" s="9" t="n"/>
     </row>
-    <row customHeight="1" ht="50" r="45">
+    <row r="45" ht="50" customHeight="1">
       <c r="A45" s="9" t="n"/>
       <c r="B45" s="9" t="n"/>
       <c r="C45" s="9" t="n"/>
@@ -16405,7 +16405,7 @@
       <c r="F45" s="9" t="n"/>
       <c r="G45" s="9" t="n"/>
     </row>
-    <row customHeight="1" ht="50" r="46">
+    <row r="46" ht="50" customHeight="1">
       <c r="A46" s="9" t="n"/>
       <c r="B46" s="9" t="n"/>
       <c r="C46" s="9" t="n"/>
@@ -16414,7 +16414,7 @@
       <c r="F46" s="9" t="n"/>
       <c r="G46" s="9" t="n"/>
     </row>
-    <row customHeight="1" ht="50" r="47">
+    <row r="47" ht="50" customHeight="1">
       <c r="A47" s="9" t="n"/>
       <c r="B47" s="9" t="n"/>
       <c r="C47" s="9" t="n"/>
@@ -16423,7 +16423,7 @@
       <c r="F47" s="9" t="n"/>
       <c r="G47" s="9" t="n"/>
     </row>
-    <row customHeight="1" ht="50" r="48">
+    <row r="48" ht="50" customHeight="1">
       <c r="A48" s="9" t="n"/>
       <c r="B48" s="9" t="n"/>
       <c r="C48" s="9" t="n"/>
@@ -16432,7 +16432,7 @@
       <c r="F48" s="9" t="n"/>
       <c r="G48" s="9" t="n"/>
     </row>
-    <row customHeight="1" ht="50" r="49">
+    <row r="49" ht="50" customHeight="1">
       <c r="A49" s="9" t="n"/>
       <c r="B49" s="9" t="n"/>
       <c r="C49" s="9" t="n"/>
@@ -16441,7 +16441,7 @@
       <c r="F49" s="9" t="n"/>
       <c r="G49" s="9" t="n"/>
     </row>
-    <row customHeight="1" ht="50" r="50">
+    <row r="50" ht="50" customHeight="1">
       <c r="A50" s="9" t="n"/>
       <c r="B50" s="9" t="n"/>
       <c r="C50" s="9" t="n"/>
@@ -16451,8 +16451,8 @@
       <c r="G50" s="9" t="n"/>
     </row>
   </sheetData>
-  <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
-  <drawing r:id="rId1"/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <drawing xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -16470,36 +16470,36 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <cols>
-    <col customWidth="1" max="1" min="1" width="15"/>
-    <col customWidth="1" max="2" min="2" width="15"/>
-    <col customWidth="1" max="3" min="3" width="10"/>
-    <col customWidth="1" max="4" min="4" width="10"/>
-    <col customWidth="1" max="5" min="5" width="10"/>
-    <col customWidth="1" max="6" min="6" width="10"/>
-    <col customWidth="1" max="7" min="7" width="10"/>
-    <col customWidth="1" max="8" min="8" width="10"/>
-    <col customWidth="1" max="9" min="9" width="10"/>
-    <col customWidth="1" max="10" min="10" width="10"/>
-    <col customWidth="1" max="11" min="11" width="10"/>
-    <col customWidth="1" max="12" min="12" width="10"/>
-    <col customWidth="1" max="13" min="13" width="10"/>
-    <col customWidth="1" max="14" min="14" width="10"/>
-    <col customWidth="1" max="15" min="15" width="10"/>
-    <col customWidth="1" max="16" min="16" width="10"/>
-    <col customWidth="1" max="17" min="17" width="10"/>
-    <col customWidth="1" max="18" min="18" width="10"/>
-    <col customWidth="1" max="19" min="19" width="10"/>
-    <col customWidth="1" max="20" min="20" width="10"/>
-    <col customWidth="1" max="21" min="21" width="10"/>
-    <col customWidth="1" max="22" min="22" width="10"/>
-    <col customWidth="1" max="23" min="23" width="10"/>
-    <col customWidth="1" max="24" min="24" width="10"/>
-    <col customWidth="1" max="25" min="25" width="10"/>
-    <col customWidth="1" max="26" min="26" width="10"/>
-    <col customWidth="1" max="27" min="27" width="10"/>
-    <col customWidth="1" max="28" min="28" width="10"/>
-    <col customWidth="1" max="29" min="29" width="35"/>
-    <col customWidth="1" max="30" min="30" width="35"/>
+    <col width="15" customWidth="1" min="1" max="1"/>
+    <col width="15" customWidth="1" min="2" max="2"/>
+    <col width="10" customWidth="1" min="3" max="3"/>
+    <col width="10" customWidth="1" min="4" max="4"/>
+    <col width="10" customWidth="1" min="5" max="5"/>
+    <col width="10" customWidth="1" min="6" max="6"/>
+    <col width="10" customWidth="1" min="7" max="7"/>
+    <col width="10" customWidth="1" min="8" max="8"/>
+    <col width="10" customWidth="1" min="9" max="9"/>
+    <col width="10" customWidth="1" min="10" max="10"/>
+    <col width="10" customWidth="1" min="11" max="11"/>
+    <col width="10" customWidth="1" min="12" max="12"/>
+    <col width="10" customWidth="1" min="13" max="13"/>
+    <col width="10" customWidth="1" min="14" max="14"/>
+    <col width="10" customWidth="1" min="15" max="15"/>
+    <col width="10" customWidth="1" min="16" max="16"/>
+    <col width="10" customWidth="1" min="17" max="17"/>
+    <col width="10" customWidth="1" min="18" max="18"/>
+    <col width="10" customWidth="1" min="19" max="19"/>
+    <col width="10" customWidth="1" min="20" max="20"/>
+    <col width="10" customWidth="1" min="21" max="21"/>
+    <col width="10" customWidth="1" min="22" max="22"/>
+    <col width="10" customWidth="1" min="23" max="23"/>
+    <col width="10" customWidth="1" min="24" max="24"/>
+    <col width="10" customWidth="1" min="25" max="25"/>
+    <col width="10" customWidth="1" min="26" max="26"/>
+    <col width="10" customWidth="1" min="27" max="27"/>
+    <col width="10" customWidth="1" min="28" max="28"/>
+    <col width="35" customWidth="1" min="29" max="29"/>
+    <col width="35" customWidth="1" min="30" max="30"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -18096,7 +18096,7 @@
     <mergeCell ref="E18:N18"/>
     <mergeCell ref="O18:X18"/>
   </mergeCells>
-  <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
 
@@ -18114,38 +18114,38 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <cols>
-    <col customWidth="1" max="1" min="1" width="15"/>
-    <col customWidth="1" max="2" min="2" width="15"/>
-    <col customWidth="1" max="3" min="3" width="10"/>
-    <col customWidth="1" max="4" min="4" width="10"/>
-    <col customWidth="1" max="5" min="5" width="10"/>
-    <col customWidth="1" max="6" min="6" width="10"/>
-    <col customWidth="1" max="7" min="7" width="10"/>
-    <col customWidth="1" max="8" min="8" width="10"/>
-    <col customWidth="1" max="9" min="9" width="10"/>
-    <col customWidth="1" max="10" min="10" width="10"/>
-    <col customWidth="1" max="11" min="11" width="10"/>
-    <col customWidth="1" max="12" min="12" width="10"/>
-    <col customWidth="1" max="13" min="13" width="10"/>
-    <col customWidth="1" max="14" min="14" width="10"/>
-    <col customWidth="1" max="15" min="15" width="10"/>
-    <col customWidth="1" max="16" min="16" width="10"/>
-    <col customWidth="1" max="17" min="17" width="10"/>
-    <col customWidth="1" max="18" min="18" width="10"/>
-    <col customWidth="1" max="19" min="19" width="10"/>
-    <col customWidth="1" max="20" min="20" width="10"/>
-    <col customWidth="1" max="21" min="21" width="10"/>
-    <col customWidth="1" max="22" min="22" width="10"/>
-    <col customWidth="1" max="23" min="23" width="10"/>
-    <col customWidth="1" max="24" min="24" width="10"/>
-    <col customWidth="1" max="25" min="25" width="10"/>
-    <col customWidth="1" max="26" min="26" width="10"/>
-    <col customWidth="1" max="27" min="27" width="10"/>
-    <col customWidth="1" max="28" min="28" width="10"/>
-    <col customWidth="1" max="29" min="29" width="10"/>
-    <col customWidth="1" max="30" min="30" width="10"/>
-    <col customWidth="1" max="31" min="31" width="35"/>
-    <col customWidth="1" max="32" min="32" width="35"/>
+    <col width="15" customWidth="1" min="1" max="1"/>
+    <col width="15" customWidth="1" min="2" max="2"/>
+    <col width="10" customWidth="1" min="3" max="3"/>
+    <col width="10" customWidth="1" min="4" max="4"/>
+    <col width="10" customWidth="1" min="5" max="5"/>
+    <col width="10" customWidth="1" min="6" max="6"/>
+    <col width="10" customWidth="1" min="7" max="7"/>
+    <col width="10" customWidth="1" min="8" max="8"/>
+    <col width="10" customWidth="1" min="9" max="9"/>
+    <col width="10" customWidth="1" min="10" max="10"/>
+    <col width="10" customWidth="1" min="11" max="11"/>
+    <col width="10" customWidth="1" min="12" max="12"/>
+    <col width="10" customWidth="1" min="13" max="13"/>
+    <col width="10" customWidth="1" min="14" max="14"/>
+    <col width="10" customWidth="1" min="15" max="15"/>
+    <col width="10" customWidth="1" min="16" max="16"/>
+    <col width="10" customWidth="1" min="17" max="17"/>
+    <col width="10" customWidth="1" min="18" max="18"/>
+    <col width="10" customWidth="1" min="19" max="19"/>
+    <col width="10" customWidth="1" min="20" max="20"/>
+    <col width="10" customWidth="1" min="21" max="21"/>
+    <col width="10" customWidth="1" min="22" max="22"/>
+    <col width="10" customWidth="1" min="23" max="23"/>
+    <col width="10" customWidth="1" min="24" max="24"/>
+    <col width="10" customWidth="1" min="25" max="25"/>
+    <col width="10" customWidth="1" min="26" max="26"/>
+    <col width="10" customWidth="1" min="27" max="27"/>
+    <col width="10" customWidth="1" min="28" max="28"/>
+    <col width="10" customWidth="1" min="29" max="29"/>
+    <col width="10" customWidth="1" min="30" max="30"/>
+    <col width="35" customWidth="1" min="31" max="31"/>
+    <col width="35" customWidth="1" min="32" max="32"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -19846,7 +19846,7 @@
     <mergeCell ref="E18:O18"/>
     <mergeCell ref="P18:Z18"/>
   </mergeCells>
-  <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
 
@@ -19864,31 +19864,31 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <cols>
-    <col customWidth="1" max="1" min="1" width="35"/>
-    <col customWidth="1" max="2" min="2" width="15"/>
-    <col customWidth="1" max="3" min="3" width="15"/>
-    <col customWidth="1" max="4" min="4" width="35"/>
-    <col customWidth="1" max="5" min="5" width="35"/>
-    <col customWidth="1" max="6" min="6" width="15"/>
-    <col customWidth="1" max="7" min="7" width="18"/>
-    <col customWidth="1" max="8" min="8" width="18"/>
-    <col customWidth="1" max="9" min="9" width="18"/>
-    <col customWidth="1" max="10" min="10" width="10"/>
-    <col customWidth="1" max="11" min="11" width="30"/>
-    <col customWidth="1" max="12" min="12" width="30"/>
-    <col customWidth="1" max="13" min="13" width="30"/>
-    <col customWidth="1" max="14" min="14" width="30"/>
-    <col customWidth="1" max="15" min="15" width="30"/>
-    <col customWidth="1" max="16" min="16" width="30"/>
-    <col customWidth="1" max="17" min="17" width="30"/>
-    <col customWidth="1" max="18" min="18" width="30"/>
-    <col customWidth="1" max="19" min="19" width="30"/>
-    <col customWidth="1" max="20" min="20" width="30"/>
-    <col customWidth="1" max="21" min="21" width="30"/>
-    <col customWidth="1" max="22" min="22" width="30"/>
+    <col width="35" customWidth="1" min="1" max="1"/>
+    <col width="15" customWidth="1" min="2" max="2"/>
+    <col width="15" customWidth="1" min="3" max="3"/>
+    <col width="35" customWidth="1" min="4" max="4"/>
+    <col width="35" customWidth="1" min="5" max="5"/>
+    <col width="15" customWidth="1" min="6" max="6"/>
+    <col width="18" customWidth="1" min="7" max="7"/>
+    <col width="18" customWidth="1" min="8" max="8"/>
+    <col width="18" customWidth="1" min="9" max="9"/>
+    <col width="10" customWidth="1" min="10" max="10"/>
+    <col width="30" customWidth="1" min="11" max="11"/>
+    <col width="30" customWidth="1" min="12" max="12"/>
+    <col width="30" customWidth="1" min="13" max="13"/>
+    <col width="30" customWidth="1" min="14" max="14"/>
+    <col width="30" customWidth="1" min="15" max="15"/>
+    <col width="30" customWidth="1" min="16" max="16"/>
+    <col width="30" customWidth="1" min="17" max="17"/>
+    <col width="30" customWidth="1" min="18" max="18"/>
+    <col width="30" customWidth="1" min="19" max="19"/>
+    <col width="30" customWidth="1" min="20" max="20"/>
+    <col width="30" customWidth="1" min="21" max="21"/>
+    <col width="30" customWidth="1" min="22" max="22"/>
   </cols>
   <sheetData>
-    <row customHeight="1" ht="25" r="1">
+    <row r="1" ht="25" customHeight="1">
       <c r="A1" s="1" t="inlineStr">
         <is>
           <t>Nome</t>
@@ -23182,6 +23182,6 @@
     </row>
   </sheetData>
   <autoFilter ref="A1:V31"/>
-  <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
</xml_diff>